<commit_message>
0,4 and 1(partly) done
</commit_message>
<xml_diff>
--- a/BewertungWEIT_Deutsch/WEIT_Bewertung_HA.xlsx
+++ b/BewertungWEIT_Deutsch/WEIT_Bewertung_HA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Personal\RUB2022\VAMoS\Sprachkompetenzmessung\BewertungWEIT_Deutsch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804AE656-EB8E-4AB8-8B50-680B63E1D8B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63945E29-0B0B-4678-8392-6F02AA3ADE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -606,11 +606,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -649,16 +656,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,7 +897,7 @@
   <dimension ref="A1:R198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1896,6 +1904,7 @@
       <c r="R27" s="1"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
       <c r="H28" s="1"/>
       <c r="J28" s="1"/>
       <c r="L28" s="1"/>

</xml_diff>

<commit_message>
Last 4 items left
</commit_message>
<xml_diff>
--- a/BewertungWEIT_Deutsch/WEIT_Bewertung_HA.xlsx
+++ b/BewertungWEIT_Deutsch/WEIT_Bewertung_HA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Personal\RUB2022\VAMoS\Sprachkompetenzmessung\BewertungWEIT_Deutsch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bdf333724b9168b/Code/SprachKompMess/BewertungWEIT_Deutsch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63945E29-0B0B-4678-8392-6F02AA3ADE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{63945E29-0B0B-4678-8392-6F02AA3ADE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADF65F7D-E889-4B8D-9256-68F54E6F1082}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9518" yWindow="0" windowWidth="9765" windowHeight="11363" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WEIT_GER" sheetId="1" r:id="rId1"/>
@@ -606,11 +606,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -656,16 +663,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -896,34 +904,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="55.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="58.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="1"/>
-    <col min="5" max="5" width="44.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="1"/>
-    <col min="7" max="7" width="55.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="4"/>
-    <col min="9" max="9" width="65.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="3"/>
-    <col min="11" max="11" width="63.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" style="4"/>
-    <col min="13" max="13" width="74.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="3"/>
-    <col min="15" max="15" width="77.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" style="4"/>
+    <col min="1" max="1" width="55.3984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" style="1"/>
+    <col min="3" max="3" width="58.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3984375" style="1"/>
+    <col min="5" max="5" width="44.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3984375" style="1"/>
+    <col min="7" max="7" width="55.3984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.86328125" style="4"/>
+    <col min="9" max="9" width="65.1328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.3984375" style="3"/>
+    <col min="11" max="11" width="63.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.86328125" style="4"/>
+    <col min="13" max="13" width="74.1328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.3984375" style="3"/>
+    <col min="15" max="15" width="77.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.86328125" style="4"/>
     <col min="17" max="17" width="60" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="3" customWidth="1"/>
-    <col min="19" max="16384" width="10.85546875" style="4"/>
+    <col min="18" max="18" width="11.3984375" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="10.86328125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -952,7 +961,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1008,16 +1017,25 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>89</v>
       </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>167</v>
       </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
       <c r="E3" s="4" t="s">
         <v>90</v>
       </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
       <c r="G3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1027,7 +1045,9 @@
       <c r="I3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
       <c r="K3" s="4" t="s">
         <v>91</v>
       </c>
@@ -1049,10 +1069,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>160</v>
       </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
       <c r="C4" s="4" t="s">
         <v>32</v>
       </c>
@@ -1062,10 +1085,15 @@
       <c r="E4" s="4" t="s">
         <v>92</v>
       </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
       <c r="G4" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
       <c r="I4" s="4" t="s">
         <v>33</v>
       </c>
@@ -1075,7 +1103,9 @@
       <c r="K4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="L4" s="1"/>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
       <c r="M4" s="4" t="s">
         <v>35</v>
       </c>
@@ -1093,16 +1123,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>161</v>
       </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
       <c r="C5" s="4" t="s">
         <v>168</v>
       </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
       <c r="E5" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
       <c r="G5" s="4" t="s">
         <v>38</v>
       </c>
@@ -1118,7 +1157,9 @@
       <c r="K5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="1"/>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
       <c r="M5" s="4" t="s">
         <v>41</v>
       </c>
@@ -1132,13 +1173,19 @@
       </c>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
       <c r="C6" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
       <c r="E6" s="4" t="s">
         <v>43</v>
       </c>
@@ -1148,11 +1195,15 @@
       <c r="G6" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1">
+        <v>2</v>
+      </c>
       <c r="I6" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
       <c r="K6" s="4" t="s">
         <v>171</v>
       </c>
@@ -1170,24 +1221,37 @@
       </c>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>100</v>
       </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
       <c r="C7" s="4" t="s">
         <v>101</v>
       </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
       <c r="E7" s="4" t="s">
         <v>102</v>
       </c>
+      <c r="F7" s="1">
+        <v>3</v>
+      </c>
       <c r="G7" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
       <c r="I7" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1">
+        <v>3</v>
+      </c>
       <c r="K7" s="4" t="s">
         <v>44</v>
       </c>
@@ -1205,10 +1269,13 @@
       </c>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>105</v>
       </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
       <c r="C8" s="4" t="s">
         <v>45</v>
       </c>
@@ -1218,10 +1285,15 @@
       <c r="E8" s="4" t="s">
         <v>106</v>
       </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
       <c r="G8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
       <c r="I8" s="4" t="s">
         <v>47</v>
       </c>
@@ -1249,24 +1321,37 @@
       </c>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>162</v>
       </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
       <c r="C9" s="4" t="s">
         <v>108</v>
       </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
       <c r="E9" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
       <c r="I9" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="J9" s="1"/>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
       <c r="K9" s="4" t="s">
         <v>111</v>
       </c>
@@ -1288,7 +1373,7 @@
       </c>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>53</v>
       </c>
@@ -1298,17 +1383,27 @@
       <c r="C10" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
       <c r="E10" s="4" t="s">
         <v>177</v>
       </c>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
       <c r="G10" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
       <c r="I10" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="J10" s="1"/>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
       <c r="K10" s="4" t="s">
         <v>178</v>
       </c>
@@ -1330,13 +1425,19 @@
       </c>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>163</v>
       </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
       <c r="C11" s="4" t="s">
         <v>115</v>
       </c>
+      <c r="D11" s="1">
+        <v>3</v>
+      </c>
       <c r="E11" s="4" t="s">
         <v>116</v>
       </c>
@@ -1346,11 +1447,15 @@
       <c r="G11" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1">
+        <v>2</v>
+      </c>
       <c r="I11" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="J11" s="1"/>
+      <c r="J11" s="1">
+        <v>2</v>
+      </c>
       <c r="K11" s="4" t="s">
         <v>118</v>
       </c>
@@ -1372,24 +1477,34 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>120</v>
       </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>121</v>
       </c>
+      <c r="F12" s="1">
+        <v>3</v>
+      </c>
       <c r="G12" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
       <c r="I12" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="J12" s="1"/>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
       <c r="K12" s="4" t="s">
         <v>59</v>
       </c>
@@ -1409,10 +1524,13 @@
       </c>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>163</v>
       </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
       <c r="C13" s="4" t="s">
         <v>61</v>
       </c>
@@ -1428,11 +1546,15 @@
       <c r="G13" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1">
+        <v>3</v>
+      </c>
       <c r="I13" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="J13" s="1"/>
+      <c r="J13" s="1">
+        <v>2</v>
+      </c>
       <c r="K13" s="4" t="s">
         <v>44</v>
       </c>
@@ -1458,7 +1580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>127</v>
       </c>
@@ -1474,6 +1596,9 @@
       <c r="E14" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
       <c r="G14" s="4" t="s">
         <v>65</v>
       </c>
@@ -1511,7 +1636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>129</v>
       </c>
@@ -1527,6 +1652,9 @@
       <c r="E15" s="4" t="s">
         <v>130</v>
       </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
       <c r="G15" s="4" t="s">
         <v>72</v>
       </c>
@@ -1564,10 +1692,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="B16" s="1">
+        <v>2</v>
+      </c>
       <c r="C16" s="4" t="s">
         <v>61</v>
       </c>
@@ -1583,11 +1714,15 @@
       <c r="G16" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1">
+        <v>2</v>
+      </c>
       <c r="I16" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J16" s="1"/>
+      <c r="J16" s="1">
+        <v>3</v>
+      </c>
       <c r="K16" s="4" t="s">
         <v>44</v>
       </c>
@@ -1611,7 +1746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>77</v>
       </c>
@@ -1667,7 +1802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
         <v>77</v>
       </c>
@@ -1677,6 +1812,9 @@
       <c r="C18" s="4" t="s">
         <v>138</v>
       </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
       <c r="E18" s="4" t="s">
         <v>43</v>
       </c>
@@ -1689,7 +1827,9 @@
       <c r="I18" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="J18" s="1"/>
+      <c r="J18" s="1">
+        <v>2</v>
+      </c>
       <c r="K18" s="4" t="s">
         <v>44</v>
       </c>
@@ -1713,20 +1853,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
         <v>164</v>
       </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
       <c r="C19" s="4" t="s">
         <v>141</v>
       </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
       <c r="E19" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
       <c r="G19" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
       <c r="I19" s="4" t="s">
         <v>82</v>
       </c>
@@ -1750,24 +1901,37 @@
       </c>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
         <v>165</v>
       </c>
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
       <c r="C20" s="4" t="s">
         <v>145</v>
       </c>
+      <c r="D20" s="1">
+        <v>3</v>
+      </c>
       <c r="E20" s="4" t="s">
         <v>146</v>
       </c>
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
       <c r="G20" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="H20" s="1"/>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
       <c r="I20" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="J20" s="1"/>
+      <c r="J20" s="1">
+        <v>2</v>
+      </c>
       <c r="K20" s="4" t="s">
         <v>148</v>
       </c>
@@ -1785,24 +1949,37 @@
       </c>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
       <c r="C21" s="4" t="s">
         <v>152</v>
       </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
       <c r="E21" s="4" t="s">
         <v>153</v>
       </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
       <c r="G21" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H21" s="1"/>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
       <c r="I21" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="J21" s="1"/>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
       <c r="K21" s="4" t="s">
         <v>185</v>
       </c>
@@ -1826,24 +2003,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
         <v>166</v>
       </c>
+      <c r="B22" s="1">
+        <v>2</v>
+      </c>
       <c r="C22" s="4" t="s">
         <v>155</v>
       </c>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
       <c r="E22" s="4" t="s">
         <v>156</v>
       </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
       <c r="G22" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="H22" s="1"/>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
       <c r="I22" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="J22" s="1"/>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
       <c r="K22" s="4" t="s">
         <v>187</v>
       </c>
@@ -1863,7 +2053,7 @@
       </c>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
       <c r="H23" s="1"/>
       <c r="J23" s="1"/>
       <c r="L23" s="1"/>
@@ -1871,7 +2061,7 @@
       <c r="P23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
       <c r="H24" s="1"/>
       <c r="J24" s="1"/>
       <c r="L24" s="1"/>
@@ -1879,7 +2069,7 @@
       <c r="P24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.45">
       <c r="H25" s="1"/>
       <c r="J25" s="1"/>
       <c r="L25" s="1"/>
@@ -1887,7 +2077,7 @@
       <c r="P25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
       <c r="H26" s="1"/>
       <c r="J26" s="1"/>
       <c r="L26" s="1"/>
@@ -1895,7 +2085,7 @@
       <c r="P26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.45">
       <c r="H27" s="1"/>
       <c r="J27" s="1"/>
       <c r="L27" s="1"/>
@@ -1903,7 +2093,7 @@
       <c r="P27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A28" s="5"/>
       <c r="H28" s="1"/>
       <c r="J28" s="1"/>
@@ -1912,7 +2102,7 @@
       <c r="P28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.45">
       <c r="H29" s="1"/>
       <c r="J29" s="1"/>
       <c r="L29" s="1"/>
@@ -1920,7 +2110,7 @@
       <c r="P29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
       <c r="H30" s="1"/>
       <c r="J30" s="1"/>
       <c r="L30" s="1"/>
@@ -1928,7 +2118,7 @@
       <c r="P30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.45">
       <c r="H31" s="1"/>
       <c r="J31" s="1"/>
       <c r="L31" s="1"/>
@@ -1936,7 +2126,7 @@
       <c r="P31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
       <c r="H32" s="1"/>
       <c r="J32" s="1"/>
       <c r="L32" s="1"/>
@@ -1944,7 +2134,7 @@
       <c r="P32" s="1"/>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H33" s="1"/>
       <c r="J33" s="1"/>
       <c r="L33" s="1"/>
@@ -1952,7 +2142,7 @@
       <c r="P33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H34" s="1"/>
       <c r="J34" s="1"/>
       <c r="L34" s="1"/>
@@ -1960,7 +2150,7 @@
       <c r="P34" s="1"/>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H35" s="1"/>
       <c r="J35" s="1"/>
       <c r="L35" s="1"/>
@@ -1968,7 +2158,7 @@
       <c r="P35" s="1"/>
       <c r="R35" s="1"/>
     </row>
-    <row r="36" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H36" s="1"/>
       <c r="J36" s="1"/>
       <c r="L36" s="1"/>
@@ -1976,7 +2166,7 @@
       <c r="P36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H37" s="1"/>
       <c r="J37" s="1"/>
       <c r="L37" s="1"/>
@@ -1984,7 +2174,7 @@
       <c r="P37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H38" s="1"/>
       <c r="J38" s="1"/>
       <c r="L38" s="1"/>
@@ -1992,7 +2182,7 @@
       <c r="P38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H39" s="1"/>
       <c r="J39" s="1"/>
       <c r="L39" s="1"/>
@@ -2000,7 +2190,7 @@
       <c r="P39" s="1"/>
       <c r="R39" s="1"/>
     </row>
-    <row r="40" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H40" s="1"/>
       <c r="J40" s="1"/>
       <c r="L40" s="1"/>
@@ -2008,7 +2198,7 @@
       <c r="P40" s="1"/>
       <c r="R40" s="1"/>
     </row>
-    <row r="41" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:18" x14ac:dyDescent="0.45">
       <c r="F41" s="3"/>
       <c r="H41" s="1"/>
       <c r="J41" s="1"/>
@@ -2017,7 +2207,7 @@
       <c r="P41" s="1"/>
       <c r="R41" s="1"/>
     </row>
-    <row r="42" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H42" s="1"/>
       <c r="J42" s="1"/>
       <c r="L42" s="1"/>
@@ -2025,7 +2215,7 @@
       <c r="P42" s="1"/>
       <c r="R42" s="1"/>
     </row>
-    <row r="43" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H43" s="1"/>
       <c r="J43" s="1"/>
       <c r="L43" s="1"/>
@@ -2033,7 +2223,7 @@
       <c r="P43" s="1"/>
       <c r="R43" s="1"/>
     </row>
-    <row r="44" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H44" s="1"/>
       <c r="J44" s="1"/>
       <c r="L44" s="1"/>
@@ -2041,7 +2231,7 @@
       <c r="P44" s="1"/>
       <c r="R44" s="1"/>
     </row>
-    <row r="45" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H45" s="1"/>
       <c r="J45" s="1"/>
       <c r="L45" s="1"/>
@@ -2049,7 +2239,7 @@
       <c r="P45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H46" s="1"/>
       <c r="J46" s="1"/>
       <c r="L46" s="1"/>
@@ -2057,7 +2247,7 @@
       <c r="P46" s="1"/>
       <c r="R46" s="1"/>
     </row>
-    <row r="47" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H47" s="1"/>
       <c r="J47" s="1"/>
       <c r="L47" s="1"/>
@@ -2065,7 +2255,7 @@
       <c r="P47" s="1"/>
       <c r="R47" s="1"/>
     </row>
-    <row r="48" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H48" s="1"/>
       <c r="J48" s="1"/>
       <c r="L48" s="1"/>
@@ -2073,7 +2263,7 @@
       <c r="P48" s="1"/>
       <c r="R48" s="1"/>
     </row>
-    <row r="49" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H49" s="1"/>
       <c r="J49" s="1"/>
       <c r="L49" s="1"/>
@@ -2081,7 +2271,7 @@
       <c r="P49" s="1"/>
       <c r="R49" s="1"/>
     </row>
-    <row r="50" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H50" s="1"/>
       <c r="J50" s="1"/>
       <c r="L50" s="1"/>
@@ -2089,7 +2279,7 @@
       <c r="P50" s="1"/>
       <c r="R50" s="1"/>
     </row>
-    <row r="51" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H51" s="1"/>
       <c r="J51" s="1"/>
       <c r="L51" s="1"/>
@@ -2097,7 +2287,7 @@
       <c r="P51" s="1"/>
       <c r="R51" s="1"/>
     </row>
-    <row r="52" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H52" s="1"/>
       <c r="J52" s="1"/>
       <c r="L52" s="1"/>
@@ -2105,7 +2295,7 @@
       <c r="P52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H53" s="1"/>
       <c r="J53" s="1"/>
       <c r="L53" s="1"/>
@@ -2113,7 +2303,7 @@
       <c r="P53" s="1"/>
       <c r="R53" s="1"/>
     </row>
-    <row r="54" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H54" s="1"/>
       <c r="J54" s="1"/>
       <c r="L54" s="1"/>
@@ -2121,7 +2311,7 @@
       <c r="P54" s="1"/>
       <c r="R54" s="1"/>
     </row>
-    <row r="55" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H55" s="1"/>
       <c r="J55" s="1"/>
       <c r="L55" s="1"/>
@@ -2129,7 +2319,7 @@
       <c r="P55" s="1"/>
       <c r="R55" s="1"/>
     </row>
-    <row r="56" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H56" s="1"/>
       <c r="J56" s="1"/>
       <c r="L56" s="1"/>
@@ -2137,7 +2327,7 @@
       <c r="P56" s="1"/>
       <c r="R56" s="1"/>
     </row>
-    <row r="57" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H57" s="1"/>
       <c r="J57" s="1"/>
       <c r="L57" s="1"/>
@@ -2145,7 +2335,7 @@
       <c r="P57" s="1"/>
       <c r="R57" s="1"/>
     </row>
-    <row r="58" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H58" s="1"/>
       <c r="J58" s="1"/>
       <c r="L58" s="1"/>
@@ -2153,7 +2343,7 @@
       <c r="P58" s="1"/>
       <c r="R58" s="1"/>
     </row>
-    <row r="59" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H59" s="1"/>
       <c r="J59" s="1"/>
       <c r="L59" s="1"/>
@@ -2161,7 +2351,7 @@
       <c r="P59" s="1"/>
       <c r="R59" s="1"/>
     </row>
-    <row r="60" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H60" s="1"/>
       <c r="J60" s="1"/>
       <c r="L60" s="1"/>
@@ -2169,7 +2359,7 @@
       <c r="P60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H61" s="1"/>
       <c r="J61" s="1"/>
       <c r="L61" s="1"/>
@@ -2177,7 +2367,7 @@
       <c r="P61" s="1"/>
       <c r="R61" s="1"/>
     </row>
-    <row r="62" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H62" s="1"/>
       <c r="J62" s="1"/>
       <c r="L62" s="1"/>
@@ -2185,7 +2375,7 @@
       <c r="P62" s="1"/>
       <c r="R62" s="1"/>
     </row>
-    <row r="63" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H63" s="1"/>
       <c r="J63" s="1"/>
       <c r="L63" s="1"/>
@@ -2193,7 +2383,7 @@
       <c r="P63" s="1"/>
       <c r="R63" s="1"/>
     </row>
-    <row r="64" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H64" s="1"/>
       <c r="J64" s="1"/>
       <c r="L64" s="1"/>
@@ -2201,7 +2391,7 @@
       <c r="P64" s="1"/>
       <c r="R64" s="1"/>
     </row>
-    <row r="65" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H65" s="1"/>
       <c r="J65" s="1"/>
       <c r="L65" s="1"/>
@@ -2209,7 +2399,7 @@
       <c r="P65" s="1"/>
       <c r="R65" s="1"/>
     </row>
-    <row r="66" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H66" s="1"/>
       <c r="J66" s="1"/>
       <c r="L66" s="1"/>
@@ -2217,7 +2407,7 @@
       <c r="P66" s="1"/>
       <c r="R66" s="1"/>
     </row>
-    <row r="67" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H67" s="1"/>
       <c r="J67" s="1"/>
       <c r="L67" s="1"/>
@@ -2225,7 +2415,7 @@
       <c r="P67" s="1"/>
       <c r="R67" s="1"/>
     </row>
-    <row r="68" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H68" s="1"/>
       <c r="J68" s="1"/>
       <c r="L68" s="1"/>
@@ -2233,14 +2423,14 @@
       <c r="P68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H69" s="1"/>
       <c r="L69" s="1"/>
       <c r="N69" s="1"/>
       <c r="P69" s="1"/>
       <c r="R69" s="1"/>
     </row>
-    <row r="70" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H70" s="1"/>
       <c r="J70" s="1"/>
       <c r="L70" s="1"/>
@@ -2248,7 +2438,7 @@
       <c r="P70" s="1"/>
       <c r="R70" s="1"/>
     </row>
-    <row r="71" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H71" s="1"/>
       <c r="J71" s="1"/>
       <c r="L71" s="1"/>
@@ -2256,7 +2446,7 @@
       <c r="P71" s="1"/>
       <c r="R71" s="1"/>
     </row>
-    <row r="72" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H72" s="1"/>
       <c r="J72" s="1"/>
       <c r="L72" s="1"/>
@@ -2264,7 +2454,7 @@
       <c r="P72" s="1"/>
       <c r="R72" s="1"/>
     </row>
-    <row r="73" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H73" s="1"/>
       <c r="J73" s="1"/>
       <c r="L73" s="1"/>
@@ -2272,7 +2462,7 @@
       <c r="P73" s="1"/>
       <c r="R73" s="1"/>
     </row>
-    <row r="74" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H74" s="1"/>
       <c r="J74" s="1"/>
       <c r="L74" s="1"/>
@@ -2280,7 +2470,7 @@
       <c r="P74" s="1"/>
       <c r="R74" s="1"/>
     </row>
-    <row r="75" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H75" s="1"/>
       <c r="J75" s="1"/>
       <c r="L75" s="1"/>
@@ -2288,7 +2478,7 @@
       <c r="P75" s="1"/>
       <c r="R75" s="1"/>
     </row>
-    <row r="76" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H76" s="1"/>
       <c r="J76" s="1"/>
       <c r="L76" s="1"/>
@@ -2296,7 +2486,7 @@
       <c r="P76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H77" s="1"/>
       <c r="J77" s="1"/>
       <c r="L77" s="1"/>
@@ -2304,7 +2494,7 @@
       <c r="P77" s="1"/>
       <c r="R77" s="1"/>
     </row>
-    <row r="78" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H78" s="1"/>
       <c r="J78" s="1"/>
       <c r="L78" s="1"/>
@@ -2312,7 +2502,7 @@
       <c r="P78" s="1"/>
       <c r="R78" s="1"/>
     </row>
-    <row r="79" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H79" s="1"/>
       <c r="J79" s="1"/>
       <c r="L79" s="1"/>
@@ -2320,7 +2510,7 @@
       <c r="P79" s="1"/>
       <c r="R79" s="1"/>
     </row>
-    <row r="80" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H80" s="1"/>
       <c r="J80" s="1"/>
       <c r="L80" s="1"/>
@@ -2328,7 +2518,7 @@
       <c r="P80" s="1"/>
       <c r="R80" s="1"/>
     </row>
-    <row r="81" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H81" s="1"/>
       <c r="J81" s="1"/>
       <c r="L81" s="1"/>
@@ -2336,14 +2526,14 @@
       <c r="P81" s="1"/>
       <c r="R81" s="1"/>
     </row>
-    <row r="82" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H82" s="1"/>
       <c r="L82" s="1"/>
       <c r="N82" s="1"/>
       <c r="P82" s="1"/>
       <c r="R82" s="1"/>
     </row>
-    <row r="83" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H83" s="1"/>
       <c r="J83" s="1"/>
       <c r="L83" s="1"/>
@@ -2351,7 +2541,7 @@
       <c r="P83" s="1"/>
       <c r="R83" s="1"/>
     </row>
-    <row r="84" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H84" s="1"/>
       <c r="J84" s="1"/>
       <c r="L84" s="1"/>
@@ -2359,7 +2549,7 @@
       <c r="P84" s="1"/>
       <c r="R84" s="1"/>
     </row>
-    <row r="85" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H85" s="1"/>
       <c r="J85" s="1"/>
       <c r="L85" s="1"/>
@@ -2367,7 +2557,7 @@
       <c r="P85" s="1"/>
       <c r="R85" s="1"/>
     </row>
-    <row r="86" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H86" s="1"/>
       <c r="J86" s="1"/>
       <c r="L86" s="1"/>
@@ -2375,7 +2565,7 @@
       <c r="P86" s="1"/>
       <c r="R86" s="1"/>
     </row>
-    <row r="87" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H87" s="1"/>
       <c r="J87" s="1"/>
       <c r="L87" s="1"/>
@@ -2383,7 +2573,7 @@
       <c r="P87" s="1"/>
       <c r="R87" s="1"/>
     </row>
-    <row r="88" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H88" s="1"/>
       <c r="J88" s="1"/>
       <c r="L88" s="1"/>
@@ -2391,7 +2581,7 @@
       <c r="P88" s="1"/>
       <c r="R88" s="1"/>
     </row>
-    <row r="89" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H89" s="1"/>
       <c r="J89" s="1"/>
       <c r="L89" s="1"/>
@@ -2399,7 +2589,7 @@
       <c r="P89" s="1"/>
       <c r="R89" s="1"/>
     </row>
-    <row r="90" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H90" s="1"/>
       <c r="J90" s="1"/>
       <c r="L90" s="1"/>
@@ -2407,7 +2597,7 @@
       <c r="P90" s="1"/>
       <c r="R90" s="1"/>
     </row>
-    <row r="91" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H91" s="1"/>
       <c r="J91" s="1"/>
       <c r="L91" s="1"/>
@@ -2415,7 +2605,7 @@
       <c r="P91" s="1"/>
       <c r="R91" s="1"/>
     </row>
-    <row r="92" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H92" s="1"/>
       <c r="J92" s="1"/>
       <c r="L92" s="1"/>
@@ -2423,7 +2613,7 @@
       <c r="P92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H93" s="1"/>
       <c r="J93" s="1"/>
       <c r="L93" s="1"/>
@@ -2431,7 +2621,7 @@
       <c r="P93" s="1"/>
       <c r="R93" s="1"/>
     </row>
-    <row r="94" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="94" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H94" s="1"/>
       <c r="J94" s="1"/>
       <c r="L94" s="1"/>
@@ -2439,7 +2629,7 @@
       <c r="P94" s="1"/>
       <c r="R94" s="1"/>
     </row>
-    <row r="95" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="6:18" x14ac:dyDescent="0.45">
       <c r="F95" s="3"/>
       <c r="H95" s="1"/>
       <c r="J95" s="1"/>
@@ -2448,7 +2638,7 @@
       <c r="P95" s="1"/>
       <c r="R95" s="1"/>
     </row>
-    <row r="96" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="6:18" x14ac:dyDescent="0.45">
       <c r="H96" s="1"/>
       <c r="J96" s="1"/>
       <c r="L96" s="1"/>
@@ -2456,7 +2646,7 @@
       <c r="P96" s="1"/>
       <c r="R96" s="1"/>
     </row>
-    <row r="97" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="97" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H97" s="1"/>
       <c r="J97" s="1"/>
       <c r="L97" s="1"/>
@@ -2464,7 +2654,7 @@
       <c r="P97" s="1"/>
       <c r="R97" s="1"/>
     </row>
-    <row r="98" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H98" s="1"/>
       <c r="J98" s="1"/>
       <c r="L98" s="1"/>
@@ -2472,7 +2662,7 @@
       <c r="P98" s="1"/>
       <c r="R98" s="1"/>
     </row>
-    <row r="99" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H99" s="1"/>
       <c r="J99" s="1"/>
       <c r="L99" s="1"/>
@@ -2480,7 +2670,7 @@
       <c r="P99" s="1"/>
       <c r="R99" s="1"/>
     </row>
-    <row r="100" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H100" s="1"/>
       <c r="J100" s="1"/>
       <c r="L100" s="1"/>
@@ -2488,7 +2678,7 @@
       <c r="P100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H101" s="1"/>
       <c r="J101" s="1"/>
       <c r="L101" s="1"/>
@@ -2496,7 +2686,7 @@
       <c r="P101" s="1"/>
       <c r="R101" s="1"/>
     </row>
-    <row r="102" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H102" s="1"/>
       <c r="J102" s="1"/>
       <c r="L102" s="1"/>
@@ -2504,7 +2694,7 @@
       <c r="P102" s="1"/>
       <c r="R102" s="1"/>
     </row>
-    <row r="103" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="103" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H103" s="1"/>
       <c r="J103" s="1"/>
       <c r="L103" s="1"/>
@@ -2512,7 +2702,7 @@
       <c r="P103" s="1"/>
       <c r="R103" s="1"/>
     </row>
-    <row r="104" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="104" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H104" s="1"/>
       <c r="J104" s="1"/>
       <c r="L104" s="1"/>
@@ -2520,7 +2710,7 @@
       <c r="P104" s="1"/>
       <c r="R104" s="1"/>
     </row>
-    <row r="105" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H105" s="1"/>
       <c r="J105" s="1"/>
       <c r="L105" s="1"/>
@@ -2528,7 +2718,7 @@
       <c r="P105" s="1"/>
       <c r="R105" s="1"/>
     </row>
-    <row r="106" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="106" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H106" s="1"/>
       <c r="J106" s="1"/>
       <c r="L106" s="1"/>
@@ -2536,7 +2726,7 @@
       <c r="P106" s="1"/>
       <c r="R106" s="1"/>
     </row>
-    <row r="107" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H107" s="1"/>
       <c r="J107" s="1"/>
       <c r="L107" s="1"/>
@@ -2544,7 +2734,7 @@
       <c r="P107" s="1"/>
       <c r="R107" s="1"/>
     </row>
-    <row r="108" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="108" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H108" s="1"/>
       <c r="J108" s="1"/>
       <c r="L108" s="1"/>
@@ -2552,7 +2742,7 @@
       <c r="P108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="109" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H109" s="1"/>
       <c r="J109" s="1"/>
       <c r="L109" s="1"/>
@@ -2560,7 +2750,7 @@
       <c r="P109" s="1"/>
       <c r="R109" s="1"/>
     </row>
-    <row r="110" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="110" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H110" s="1"/>
       <c r="J110" s="1"/>
       <c r="L110" s="1"/>
@@ -2568,7 +2758,7 @@
       <c r="P110" s="1"/>
       <c r="R110" s="1"/>
     </row>
-    <row r="111" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="111" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H111" s="1"/>
       <c r="J111" s="1"/>
       <c r="L111" s="1"/>
@@ -2576,7 +2766,7 @@
       <c r="P111" s="1"/>
       <c r="R111" s="1"/>
     </row>
-    <row r="112" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="112" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H112" s="1"/>
       <c r="J112" s="1"/>
       <c r="L112" s="1"/>
@@ -2584,7 +2774,7 @@
       <c r="P112" s="1"/>
       <c r="R112" s="1"/>
     </row>
-    <row r="113" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="113" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H113" s="1"/>
       <c r="J113" s="1"/>
       <c r="L113" s="1"/>
@@ -2592,7 +2782,7 @@
       <c r="P113" s="1"/>
       <c r="R113" s="1"/>
     </row>
-    <row r="114" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="114" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H114" s="1"/>
       <c r="J114" s="1"/>
       <c r="L114" s="1"/>
@@ -2600,7 +2790,7 @@
       <c r="P114" s="1"/>
       <c r="R114" s="1"/>
     </row>
-    <row r="115" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="115" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H115" s="1"/>
       <c r="J115" s="1"/>
       <c r="L115" s="1"/>
@@ -2608,7 +2798,7 @@
       <c r="P115" s="1"/>
       <c r="R115" s="1"/>
     </row>
-    <row r="116" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="116" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H116" s="1"/>
       <c r="J116" s="1"/>
       <c r="L116" s="1"/>
@@ -2616,7 +2806,7 @@
       <c r="P116" s="1"/>
       <c r="R116" s="1"/>
     </row>
-    <row r="117" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="117" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H117" s="1"/>
       <c r="J117" s="1"/>
       <c r="L117" s="1"/>
@@ -2624,7 +2814,7 @@
       <c r="P117" s="1"/>
       <c r="R117" s="1"/>
     </row>
-    <row r="118" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="118" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H118" s="1"/>
       <c r="J118" s="1"/>
       <c r="L118" s="1"/>
@@ -2632,7 +2822,7 @@
       <c r="P118" s="1"/>
       <c r="R118" s="1"/>
     </row>
-    <row r="119" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="119" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H119" s="1"/>
       <c r="J119" s="1"/>
       <c r="L119" s="1"/>
@@ -2640,7 +2830,7 @@
       <c r="P119" s="1"/>
       <c r="R119" s="1"/>
     </row>
-    <row r="120" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="120" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H120" s="1"/>
       <c r="J120" s="1"/>
       <c r="L120" s="1"/>
@@ -2648,7 +2838,7 @@
       <c r="P120" s="1"/>
       <c r="R120" s="1"/>
     </row>
-    <row r="121" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="121" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H121" s="1"/>
       <c r="J121" s="1"/>
       <c r="L121" s="1"/>
@@ -2656,7 +2846,7 @@
       <c r="P121" s="1"/>
       <c r="R121" s="1"/>
     </row>
-    <row r="122" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="122" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H122" s="1"/>
       <c r="J122" s="1"/>
       <c r="L122" s="1"/>
@@ -2664,7 +2854,7 @@
       <c r="P122" s="1"/>
       <c r="R122" s="1"/>
     </row>
-    <row r="123" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="123" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H123" s="1"/>
       <c r="J123" s="1"/>
       <c r="L123" s="1"/>
@@ -2672,7 +2862,7 @@
       <c r="P123" s="1"/>
       <c r="R123" s="1"/>
     </row>
-    <row r="124" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="124" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H124" s="1"/>
       <c r="J124" s="1"/>
       <c r="L124" s="1"/>
@@ -2680,7 +2870,7 @@
       <c r="P124" s="1"/>
       <c r="R124" s="1"/>
     </row>
-    <row r="125" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="125" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H125" s="1"/>
       <c r="J125" s="1"/>
       <c r="L125" s="1"/>
@@ -2688,7 +2878,7 @@
       <c r="P125" s="1"/>
       <c r="R125" s="1"/>
     </row>
-    <row r="126" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="126" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H126" s="1"/>
       <c r="J126" s="1"/>
       <c r="L126" s="1"/>
@@ -2696,7 +2886,7 @@
       <c r="P126" s="1"/>
       <c r="R126" s="1"/>
     </row>
-    <row r="127" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="127" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H127" s="1"/>
       <c r="J127" s="1"/>
       <c r="L127" s="1"/>
@@ -2704,7 +2894,7 @@
       <c r="P127" s="1"/>
       <c r="R127" s="1"/>
     </row>
-    <row r="128" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="128" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H128" s="1"/>
       <c r="J128" s="1"/>
       <c r="L128" s="1"/>
@@ -2712,7 +2902,7 @@
       <c r="P128" s="1"/>
       <c r="R128" s="1"/>
     </row>
-    <row r="129" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="129" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H129" s="1"/>
       <c r="J129" s="1"/>
       <c r="L129" s="1"/>
@@ -2720,7 +2910,7 @@
       <c r="P129" s="1"/>
       <c r="R129" s="1"/>
     </row>
-    <row r="130" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="130" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H130" s="1"/>
       <c r="J130" s="1"/>
       <c r="L130" s="1"/>
@@ -2728,7 +2918,7 @@
       <c r="P130" s="1"/>
       <c r="R130" s="1"/>
     </row>
-    <row r="131" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="131" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H131" s="1"/>
       <c r="J131" s="1"/>
       <c r="L131" s="1"/>
@@ -2736,7 +2926,7 @@
       <c r="P131" s="1"/>
       <c r="R131" s="1"/>
     </row>
-    <row r="132" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="132" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H132" s="1"/>
       <c r="J132" s="1"/>
       <c r="L132" s="1"/>
@@ -2744,7 +2934,7 @@
       <c r="P132" s="1"/>
       <c r="R132" s="1"/>
     </row>
-    <row r="133" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="133" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H133" s="1"/>
       <c r="J133" s="1"/>
       <c r="L133" s="1"/>
@@ -2752,7 +2942,7 @@
       <c r="P133" s="1"/>
       <c r="R133" s="1"/>
     </row>
-    <row r="134" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="134" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H134" s="1"/>
       <c r="J134" s="1"/>
       <c r="L134" s="1"/>
@@ -2760,7 +2950,7 @@
       <c r="P134" s="1"/>
       <c r="R134" s="1"/>
     </row>
-    <row r="135" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="135" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H135" s="1"/>
       <c r="J135" s="1"/>
       <c r="L135" s="1"/>
@@ -2768,7 +2958,7 @@
       <c r="P135" s="1"/>
       <c r="R135" s="1"/>
     </row>
-    <row r="136" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="136" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H136" s="1"/>
       <c r="J136" s="1"/>
       <c r="L136" s="1"/>
@@ -2776,7 +2966,7 @@
       <c r="P136" s="1"/>
       <c r="R136" s="1"/>
     </row>
-    <row r="137" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="137" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H137" s="1"/>
       <c r="J137" s="1"/>
       <c r="L137" s="1"/>
@@ -2784,7 +2974,7 @@
       <c r="P137" s="1"/>
       <c r="R137" s="1"/>
     </row>
-    <row r="138" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="138" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H138" s="1"/>
       <c r="J138" s="1"/>
       <c r="L138" s="1"/>
@@ -2792,7 +2982,7 @@
       <c r="P138" s="1"/>
       <c r="R138" s="1"/>
     </row>
-    <row r="139" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="139" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H139" s="1"/>
       <c r="J139" s="1"/>
       <c r="L139" s="1"/>
@@ -2800,7 +2990,7 @@
       <c r="P139" s="1"/>
       <c r="R139" s="1"/>
     </row>
-    <row r="140" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="140" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H140" s="1"/>
       <c r="J140" s="1"/>
       <c r="L140" s="1"/>
@@ -2808,7 +2998,7 @@
       <c r="P140" s="1"/>
       <c r="R140" s="1"/>
     </row>
-    <row r="141" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="141" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H141" s="1"/>
       <c r="J141" s="1"/>
       <c r="L141" s="1"/>
@@ -2816,7 +3006,7 @@
       <c r="P141" s="1"/>
       <c r="R141" s="1"/>
     </row>
-    <row r="142" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="142" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H142" s="1"/>
       <c r="J142" s="1"/>
       <c r="L142" s="1"/>
@@ -2824,7 +3014,7 @@
       <c r="P142" s="1"/>
       <c r="R142" s="1"/>
     </row>
-    <row r="143" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="143" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H143" s="1"/>
       <c r="J143" s="1"/>
       <c r="L143" s="1"/>
@@ -2832,7 +3022,7 @@
       <c r="P143" s="1"/>
       <c r="R143" s="1"/>
     </row>
-    <row r="144" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="144" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H144" s="1"/>
       <c r="J144" s="1"/>
       <c r="L144" s="1"/>
@@ -2840,7 +3030,7 @@
       <c r="P144" s="1"/>
       <c r="R144" s="1"/>
     </row>
-    <row r="145" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="145" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H145" s="1"/>
       <c r="J145" s="1"/>
       <c r="L145" s="1"/>
@@ -2848,7 +3038,7 @@
       <c r="P145" s="1"/>
       <c r="R145" s="1"/>
     </row>
-    <row r="146" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="146" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H146" s="1"/>
       <c r="J146" s="1"/>
       <c r="L146" s="1"/>
@@ -2856,7 +3046,7 @@
       <c r="P146" s="1"/>
       <c r="R146" s="1"/>
     </row>
-    <row r="147" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="147" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H147" s="1"/>
       <c r="J147" s="1"/>
       <c r="L147" s="1"/>
@@ -2864,7 +3054,7 @@
       <c r="P147" s="1"/>
       <c r="R147" s="1"/>
     </row>
-    <row r="148" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="148" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H148" s="1"/>
       <c r="J148" s="1"/>
       <c r="L148" s="1"/>
@@ -2872,14 +3062,14 @@
       <c r="P148" s="1"/>
       <c r="R148" s="1"/>
     </row>
-    <row r="149" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="149" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H149" s="1"/>
       <c r="L149" s="1"/>
       <c r="N149" s="1"/>
       <c r="P149" s="1"/>
       <c r="R149" s="1"/>
     </row>
-    <row r="150" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="150" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H150" s="1"/>
       <c r="J150" s="1"/>
       <c r="L150" s="1"/>
@@ -2887,7 +3077,7 @@
       <c r="P150" s="1"/>
       <c r="R150" s="1"/>
     </row>
-    <row r="151" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="151" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H151" s="1"/>
       <c r="J151" s="1"/>
       <c r="L151" s="1"/>
@@ -2895,7 +3085,7 @@
       <c r="P151" s="1"/>
       <c r="R151" s="1"/>
     </row>
-    <row r="152" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="152" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H152" s="1"/>
       <c r="J152" s="1"/>
       <c r="L152" s="1"/>
@@ -2903,7 +3093,7 @@
       <c r="P152" s="1"/>
       <c r="R152" s="1"/>
     </row>
-    <row r="153" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="153" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H153" s="1"/>
       <c r="J153" s="1"/>
       <c r="L153" s="1"/>
@@ -2911,7 +3101,7 @@
       <c r="P153" s="1"/>
       <c r="R153" s="1"/>
     </row>
-    <row r="154" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="154" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H154" s="1"/>
       <c r="J154" s="1"/>
       <c r="L154" s="1"/>
@@ -2919,7 +3109,7 @@
       <c r="P154" s="1"/>
       <c r="R154" s="1"/>
     </row>
-    <row r="155" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="155" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H155" s="1"/>
       <c r="J155" s="1"/>
       <c r="L155" s="1"/>
@@ -2927,7 +3117,7 @@
       <c r="P155" s="1"/>
       <c r="R155" s="1"/>
     </row>
-    <row r="156" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="156" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H156" s="1"/>
       <c r="J156" s="1"/>
       <c r="L156" s="1"/>
@@ -2935,7 +3125,7 @@
       <c r="P156" s="1"/>
       <c r="R156" s="1"/>
     </row>
-    <row r="157" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="157" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H157" s="1"/>
       <c r="J157" s="1"/>
       <c r="L157" s="1"/>
@@ -2943,7 +3133,7 @@
       <c r="P157" s="1"/>
       <c r="R157" s="1"/>
     </row>
-    <row r="158" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="158" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H158" s="1"/>
       <c r="J158" s="1"/>
       <c r="L158" s="1"/>
@@ -2951,7 +3141,7 @@
       <c r="P158" s="1"/>
       <c r="R158" s="1"/>
     </row>
-    <row r="159" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="159" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H159" s="1"/>
       <c r="J159" s="1"/>
       <c r="L159" s="1"/>
@@ -2959,7 +3149,7 @@
       <c r="P159" s="1"/>
       <c r="R159" s="1"/>
     </row>
-    <row r="160" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="160" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H160" s="1"/>
       <c r="J160" s="1"/>
       <c r="L160" s="1"/>
@@ -2967,7 +3157,7 @@
       <c r="P160" s="1"/>
       <c r="R160" s="1"/>
     </row>
-    <row r="161" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="161" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H161" s="1"/>
       <c r="J161" s="1"/>
       <c r="L161" s="1"/>
@@ -2975,7 +3165,7 @@
       <c r="P161" s="1"/>
       <c r="R161" s="1"/>
     </row>
-    <row r="162" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="162" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H162" s="1"/>
       <c r="J162" s="1"/>
       <c r="L162" s="1"/>
@@ -2983,7 +3173,7 @@
       <c r="P162" s="1"/>
       <c r="R162" s="1"/>
     </row>
-    <row r="163" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="163" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H163" s="1"/>
       <c r="J163" s="1"/>
       <c r="L163" s="1"/>
@@ -2991,7 +3181,7 @@
       <c r="P163" s="1"/>
       <c r="R163" s="1"/>
     </row>
-    <row r="164" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="164" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H164" s="1"/>
       <c r="J164" s="1"/>
       <c r="L164" s="1"/>
@@ -2999,7 +3189,7 @@
       <c r="P164" s="1"/>
       <c r="R164" s="1"/>
     </row>
-    <row r="165" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="165" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H165" s="1"/>
       <c r="J165" s="1"/>
       <c r="L165" s="1"/>
@@ -3007,7 +3197,7 @@
       <c r="P165" s="1"/>
       <c r="R165" s="1"/>
     </row>
-    <row r="166" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="166" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H166" s="1"/>
       <c r="J166" s="1"/>
       <c r="L166" s="1"/>
@@ -3015,7 +3205,7 @@
       <c r="P166" s="1"/>
       <c r="R166" s="1"/>
     </row>
-    <row r="167" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="167" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H167" s="1"/>
       <c r="J167" s="1"/>
       <c r="L167" s="1"/>
@@ -3023,7 +3213,7 @@
       <c r="P167" s="1"/>
       <c r="R167" s="1"/>
     </row>
-    <row r="168" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="168" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H168" s="1"/>
       <c r="J168" s="1"/>
       <c r="L168" s="1"/>
@@ -3031,7 +3221,7 @@
       <c r="P168" s="1"/>
       <c r="R168" s="1"/>
     </row>
-    <row r="169" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="169" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H169" s="1"/>
       <c r="J169" s="1"/>
       <c r="L169" s="1"/>
@@ -3039,7 +3229,7 @@
       <c r="P169" s="1"/>
       <c r="R169" s="1"/>
     </row>
-    <row r="170" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="170" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H170" s="1"/>
       <c r="J170" s="1"/>
       <c r="L170" s="1"/>
@@ -3047,7 +3237,7 @@
       <c r="P170" s="1"/>
       <c r="R170" s="1"/>
     </row>
-    <row r="171" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="171" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H171" s="1"/>
       <c r="J171" s="1"/>
       <c r="L171" s="1"/>
@@ -3055,7 +3245,7 @@
       <c r="P171" s="1"/>
       <c r="R171" s="1"/>
     </row>
-    <row r="172" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="172" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H172" s="1"/>
       <c r="J172" s="1"/>
       <c r="L172" s="1"/>
@@ -3063,7 +3253,7 @@
       <c r="P172" s="1"/>
       <c r="R172" s="1"/>
     </row>
-    <row r="173" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="173" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H173" s="1"/>
       <c r="J173" s="1"/>
       <c r="L173" s="1"/>
@@ -3071,7 +3261,7 @@
       <c r="P173" s="1"/>
       <c r="R173" s="1"/>
     </row>
-    <row r="174" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="174" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H174" s="1"/>
       <c r="J174" s="1"/>
       <c r="L174" s="1"/>
@@ -3079,7 +3269,7 @@
       <c r="P174" s="1"/>
       <c r="R174" s="1"/>
     </row>
-    <row r="175" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="175" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H175" s="1"/>
       <c r="J175" s="1"/>
       <c r="L175" s="1"/>
@@ -3087,7 +3277,7 @@
       <c r="P175" s="1"/>
       <c r="R175" s="1"/>
     </row>
-    <row r="176" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="176" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H176" s="1"/>
       <c r="J176" s="1"/>
       <c r="L176" s="1"/>
@@ -3095,7 +3285,7 @@
       <c r="P176" s="1"/>
       <c r="R176" s="1"/>
     </row>
-    <row r="177" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="177" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H177" s="1"/>
       <c r="J177" s="1"/>
       <c r="L177" s="1"/>
@@ -3103,7 +3293,7 @@
       <c r="P177" s="1"/>
       <c r="R177" s="1"/>
     </row>
-    <row r="178" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="178" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H178" s="1"/>
       <c r="J178" s="1"/>
       <c r="L178" s="1"/>
@@ -3111,7 +3301,7 @@
       <c r="P178" s="1"/>
       <c r="R178" s="1"/>
     </row>
-    <row r="179" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="179" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H179" s="1"/>
       <c r="J179" s="1"/>
       <c r="L179" s="1"/>
@@ -3119,7 +3309,7 @@
       <c r="P179" s="1"/>
       <c r="R179" s="1"/>
     </row>
-    <row r="180" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="180" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H180" s="1"/>
       <c r="J180" s="1"/>
       <c r="L180" s="1"/>
@@ -3127,7 +3317,7 @@
       <c r="P180" s="1"/>
       <c r="R180" s="1"/>
     </row>
-    <row r="181" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="181" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H181" s="1"/>
       <c r="J181" s="1"/>
       <c r="L181" s="1"/>
@@ -3135,7 +3325,7 @@
       <c r="P181" s="1"/>
       <c r="R181" s="1"/>
     </row>
-    <row r="182" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="182" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H182" s="1"/>
       <c r="J182" s="1"/>
       <c r="L182" s="1"/>
@@ -3143,7 +3333,7 @@
       <c r="P182" s="1"/>
       <c r="R182" s="1"/>
     </row>
-    <row r="183" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="183" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H183" s="1"/>
       <c r="J183" s="1"/>
       <c r="L183" s="1"/>
@@ -3151,7 +3341,7 @@
       <c r="P183" s="1"/>
       <c r="R183" s="1"/>
     </row>
-    <row r="184" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="184" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H184" s="1"/>
       <c r="J184" s="1"/>
       <c r="L184" s="1"/>
@@ -3159,7 +3349,7 @@
       <c r="P184" s="1"/>
       <c r="R184" s="1"/>
     </row>
-    <row r="185" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="185" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H185" s="1"/>
       <c r="J185" s="1"/>
       <c r="L185" s="1"/>
@@ -3167,7 +3357,7 @@
       <c r="P185" s="1"/>
       <c r="R185" s="1"/>
     </row>
-    <row r="186" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="186" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H186" s="1"/>
       <c r="J186" s="1"/>
       <c r="L186" s="1"/>
@@ -3175,7 +3365,7 @@
       <c r="P186" s="1"/>
       <c r="R186" s="1"/>
     </row>
-    <row r="187" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="187" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H187" s="1"/>
       <c r="J187" s="1"/>
       <c r="L187" s="1"/>
@@ -3183,7 +3373,7 @@
       <c r="P187" s="1"/>
       <c r="R187" s="1"/>
     </row>
-    <row r="188" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="188" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H188" s="1"/>
       <c r="J188" s="1"/>
       <c r="L188" s="1"/>
@@ -3191,7 +3381,7 @@
       <c r="P188" s="1"/>
       <c r="R188" s="1"/>
     </row>
-    <row r="189" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="189" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H189" s="1"/>
       <c r="J189" s="1"/>
       <c r="L189" s="1"/>
@@ -3199,7 +3389,7 @@
       <c r="P189" s="1"/>
       <c r="R189" s="1"/>
     </row>
-    <row r="190" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="190" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H190" s="1"/>
       <c r="J190" s="1"/>
       <c r="L190" s="1"/>
@@ -3207,7 +3397,7 @@
       <c r="P190" s="1"/>
       <c r="R190" s="1"/>
     </row>
-    <row r="191" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="191" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H191" s="1"/>
       <c r="J191" s="1"/>
       <c r="L191" s="1"/>
@@ -3215,7 +3405,7 @@
       <c r="P191" s="1"/>
       <c r="R191" s="1"/>
     </row>
-    <row r="192" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="192" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H192" s="1"/>
       <c r="J192" s="1"/>
       <c r="L192" s="1"/>
@@ -3223,7 +3413,7 @@
       <c r="P192" s="1"/>
       <c r="R192" s="1"/>
     </row>
-    <row r="193" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="193" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H193" s="1"/>
       <c r="J193" s="1"/>
       <c r="L193" s="1"/>
@@ -3231,7 +3421,7 @@
       <c r="P193" s="1"/>
       <c r="R193" s="1"/>
     </row>
-    <row r="194" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="194" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H194" s="1"/>
       <c r="J194" s="1"/>
       <c r="L194" s="1"/>
@@ -3239,7 +3429,7 @@
       <c r="P194" s="1"/>
       <c r="R194" s="1"/>
     </row>
-    <row r="195" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="195" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H195" s="1"/>
       <c r="J195" s="1"/>
       <c r="L195" s="1"/>
@@ -3247,7 +3437,7 @@
       <c r="P195" s="1"/>
       <c r="R195" s="1"/>
     </row>
-    <row r="196" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="196" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H196" s="1"/>
       <c r="J196" s="1"/>
       <c r="L196" s="1"/>
@@ -3255,7 +3445,7 @@
       <c r="P196" s="1"/>
       <c r="R196" s="1"/>
     </row>
-    <row r="197" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="197" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H197" s="1"/>
       <c r="J197" s="1"/>
       <c r="L197" s="1"/>
@@ -3263,7 +3453,7 @@
       <c r="P197" s="1"/>
       <c r="R197" s="1"/>
     </row>
-    <row r="198" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="198" spans="8:18" x14ac:dyDescent="0.45">
       <c r="H198" s="1"/>
       <c r="J198" s="1"/>
       <c r="L198" s="1"/>

</xml_diff>